<commit_message>
Finished Mobile automation final push.
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/Mobile_Data.xlsx
+++ b/src/main/java/resources/excelsheet/Mobile_Data.xlsx
@@ -414,10 +414,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>